<commit_message>
New code layout, new filenames
Changed code strategy from class, to global functions. Doesn't work!
</commit_message>
<xml_diff>
--- a/Data_Fourier Analysis/Data/M75_T1.xlsx
+++ b/Data_Fourier Analysis/Data/M75_T1.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="M75_T1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -854,7 +854,7 @@
   <dimension ref="A1:G1893"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>